<commit_message>
update model and emb analysis
</commit_message>
<xml_diff>
--- a/dataAnalysis.xlsx
+++ b/dataAnalysis.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\botImpact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4BF5EB-C8B3-4888-B735-8EAA4BD14353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1D41B4-9307-437D-80D7-C4B9CA4E2137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Model-Free" sheetId="1" r:id="rId1"/>
+    <sheet name="ModelFreeEvidence" sheetId="1" r:id="rId1"/>
     <sheet name="Sentiment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -26,11 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
-  <si>
-    <t>Topic: Pandemic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>Node Degree</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,14 +157,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Topic: War</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Topic: Climate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>H→H</t>
     </r>
@@ -369,10 +357,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Statistical Tests: Homophily amoung Neighboring Nodes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">A→B, </t>
     </r>
@@ -497,10 +481,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Treatment Effect: Naïve Approach</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -682,6 +662,384 @@
       </rPr>
       <t>Bot</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Pos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>估计</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Neg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>估计</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Pandemic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>War</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>影响大于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Human</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，而</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Climate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>小于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Human</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>差距增大，算法觉得Human的影响应该更小而Bot的影响应该更大些</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区别翻转，算法觉得Human的影响应该更小而Bot的影响应该更大些</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>因为网络更大，训练的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>需要比模拟数据更多</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>差距增大，算法觉得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Human</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>影响应该更小而</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的影响应该更大些</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>区别翻转，算法觉得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Human</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>影响应该更小而</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的影响应该更大些</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>差距增大，算法觉得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的影响应该更大些</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Threshold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：0.8, -0.8</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Topic: Pandemic [Tweet: 1208982]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Topic: War [Tweet: 2299370]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Topic: Climate [Tweet: 373795]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三个数据集表头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以再成表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表格内容可变成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柱状图(433030)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表格形式呈现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statistical Tests: Homophily among Neighboring Nodes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -692,7 +1050,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,8 +1091,77 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFCC0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC0000"/>
+      <name val="宋体"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,8 +1180,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -840,11 +1273,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -858,31 +1302,55 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -906,6 +1374,12 @@
     <xf numFmtId="176" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -915,7 +1389,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -926,6 +1406,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FFCC0000"/>
       <color rgb="FFEAFAFA"/>
       <color rgb="FFF8FEFE"/>
       <color rgb="FFE7F5F5"/>
@@ -1207,84 +1689,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="4" width="15.19921875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.546875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="20.796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" style="2" customWidth="1"/>
     <col min="5" max="7" width="10.69921875" style="2" customWidth="1"/>
     <col min="8" max="9" width="16.8984375" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A1" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A2" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17"/>
-      <c r="E1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A2" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="E2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>28</v>
+      <c r="E3" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2">
         <v>0.82099999999999995</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="29">
         <v>23.857700000000001</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I3" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2">
         <v>7.149</v>
@@ -1292,19 +1784,22 @@
       <c r="C4" s="2">
         <v>6.9372999999999996</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="D4" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="21"/>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2">
         <v>0.74229999999999996</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>3.0872000000000002</v>
@@ -1312,130 +1807,133 @@
       <c r="C5" s="2">
         <v>5.8960999999999997</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>29</v>
+      <c r="D5" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G5" s="2">
         <v>0.83950000000000002</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="29">
         <v>20.513400000000001</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="E6" s="6"/>
+      <c r="I5" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A6" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2">
         <v>0.73529999999999995</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A7" s="14" t="s">
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A7" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>30</v>
+      <c r="E7" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G7" s="2">
         <v>0.78539999999999999</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="29">
         <v>16.601400000000002</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A8" s="6"/>
+      <c r="I7" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A8" s="21"/>
       <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2">
         <v>0.67610000000000003</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A11" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="E11" s="9" t="s">
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A10" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A11" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="E11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A13" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A13" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="B13" s="2">
         <v>5.1664000000000003</v>
@@ -1443,25 +1941,25 @@
       <c r="C13" s="2">
         <v>5.0496999999999996</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>28</v>
+      <c r="E13" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G13" s="2">
         <v>0.60419999999999996</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="29">
         <v>6.7031000000000001</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I13" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="2">
         <v>2.8283</v>
@@ -1469,121 +1967,121 @@
       <c r="C14" s="2">
         <v>5.5609000000000002</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" s="2">
         <v>0.56520000000000004</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="E15" s="5" t="s">
-        <v>29</v>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A15" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="E15" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G15" s="2">
         <v>0.58009999999999995</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="29">
         <v>2.8894000000000002</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="29">
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A16" s="14" t="s">
-        <v>8</v>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A16" s="22" t="s">
+        <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="E16" s="21"/>
       <c r="F16" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G16" s="2">
         <v>0.5534</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A17" s="6"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G17" s="2">
         <v>0.5393</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="29">
         <v>1.9854000000000001</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="29">
         <v>3.7600000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="E18" s="6"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G18" s="2">
         <v>0.52139999999999997</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A19" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
+      <c r="A19" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A20" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="A20" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="2">
         <v>6.5907999999999998</v>
@@ -1594,7 +2092,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" s="2">
         <v>2.9424000000000001</v>
@@ -1604,34 +2102,52 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A25" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A25" s="14" t="s">
-        <v>8</v>
-      </c>
       <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A26" s="21"/>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A26" s="6"/>
-      <c r="B26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:E4"/>
@@ -1648,24 +2164,6 @@
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A24:C24"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1675,10 +2173,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2687A086-E6AD-4DC9-8E6D-5E9AEFD1DED8}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -1690,261 +2188,375 @@
     <col min="7" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A1" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A1" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A3" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2460</v>
+      </c>
+      <c r="D3" s="4">
+        <v>34169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4" s="21"/>
+      <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1038</v>
+      </c>
+      <c r="D4" s="4">
+        <v>17553</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4">
+        <v>777</v>
+      </c>
+      <c r="D5" s="4">
+        <v>19922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A6" s="21"/>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1267</v>
+      </c>
+      <c r="D6" s="4">
+        <v>40701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A7" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4">
+        <v>736</v>
+      </c>
+      <c r="D7" s="4">
+        <v>13377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A8" s="21"/>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4">
+        <v>227</v>
+      </c>
+      <c r="D8" s="4">
+        <v>4945</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="4">
-        <v>34169</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="4">
-        <v>17553</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="4">
-        <v>19922</v>
-      </c>
-      <c r="D5" s="4">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="4">
-        <v>40701</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1267</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="4">
-        <v>13377</v>
-      </c>
-      <c r="D7" s="4">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="4">
-        <v>4945</v>
-      </c>
-      <c r="D8" s="4">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A10" s="21" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.20519999999999999</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.1487</v>
+      </c>
+      <c r="E11" s="2">
+        <f>D11-C11</f>
+        <v>-5.6499999999999995E-2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A12" s="34"/>
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.2326</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.14749999999999999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-8.5099999999999995E-2</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A13" s="34"/>
+      <c r="B13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="9">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="D13" s="10">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <f>D13-C13</f>
+        <v>5.8400000000000001E-2</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A14" s="21"/>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="9">
+        <v>-1.2999999999999999E-3</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.1249</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.14080000000000001</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A15" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="7">
+        <v>-8.3900000000000002E-2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>-0.11269999999999999</v>
+      </c>
+      <c r="E15" s="2">
+        <f>D15-C15</f>
+        <v>-2.8799999999999992E-2</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A16" s="34"/>
+      <c r="B16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="7">
+        <v>-5.0999999999999997E-2</v>
+      </c>
+      <c r="D16" s="8">
+        <v>-0.11840000000000001</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-6.7400000000000002E-2</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A17" s="34"/>
+      <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="9">
+        <v>-0.2681</v>
+      </c>
+      <c r="D17" s="10">
+        <v>-0.17510000000000001</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D17-C17</f>
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A18" s="21"/>
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="9">
+        <v>-0.31459999999999999</v>
+      </c>
+      <c r="D18" s="10">
+        <v>-6.2700000000000006E-2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.25180000000000002</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.1537</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0.2175</v>
+      </c>
+      <c r="E19" s="2">
+        <f>D19-C19</f>
+        <v>6.3799999999999996E-2</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="4" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A20" s="34"/>
+      <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="C20" s="8">
+        <v>0.17810000000000001</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.15720000000000001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>-2.0899999999999998E-2</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A21" s="34"/>
+      <c r="B21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0.1953</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.11890000000000001</v>
+      </c>
+      <c r="E21" s="2">
+        <f>D21-C21</f>
+        <v>-7.6399999999999996E-2</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0.1487</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.20519999999999999</v>
-      </c>
-      <c r="E12" s="4">
-        <f>C12-D12</f>
-        <v>-5.6499999999999995E-2</v>
-      </c>
-      <c r="F12" s="24" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A22" s="21"/>
+      <c r="B22" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="4">
-        <v>6.1600000000000002E-2</v>
-      </c>
-      <c r="D13" s="4">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" ref="E13:E17" si="0">C13-D13</f>
-        <v>5.8400000000000001E-2</v>
-      </c>
-      <c r="F13" s="24" t="s">
+      <c r="C22" s="10">
+        <v>0.14760000000000001</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.23960000000000001</v>
+      </c>
+      <c r="E22" s="2">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C27" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="4">
-        <v>-0.11269999999999999</v>
-      </c>
-      <c r="D14" s="4">
-        <v>-8.3900000000000002E-2</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>-2.8799999999999992E-2</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="4">
-        <v>-0.17510000000000001</v>
-      </c>
-      <c r="D15" s="4">
-        <v>-0.2681</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.2175</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.1537</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>6.3799999999999996E-2</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.11890000000000001</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.1953</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="0"/>
-        <v>-7.6399999999999996E-2</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A10:D10"/>
+  <mergeCells count="7">
+    <mergeCell ref="A19:A22"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update lp running version
</commit_message>
<xml_diff>
--- a/dataAnalysis.xlsx
+++ b/dataAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\botImpact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3953190A-71CC-4EDF-BE55-2DDC939D76C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CD6EC2-F68C-4B4B-A804-7750D1596254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>Node Degree</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1064,6 +1064,42 @@
   </si>
   <si>
     <t>Effect (Bot-Human)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCN Prediction ('Positive' Influence Sources)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCN Prediction ('Negative' Influence Sources)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bot Inf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Human Inf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data / Metric</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average Inner Product</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1071,8 +1107,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1331,7 +1368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1387,6 +1424,18 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1400,12 +1449,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1429,12 +1472,6 @@
     <xf numFmtId="176" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1442,6 +1479,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1752,35 +1825,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="21"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="23"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
@@ -1804,7 +1877,7 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1813,10 +1886,10 @@
       <c r="G3" s="2">
         <v>0.82099999999999995</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="21">
         <v>23.857700000000001</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="21" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1833,15 +1906,15 @@
       <c r="D4" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="2">
         <v>0.74229999999999996</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
@@ -1856,7 +1929,7 @@
       <c r="D5" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1865,31 +1938,31 @@
       <c r="G5" s="2">
         <v>0.83950000000000002</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="21">
         <v>20.513400000000001</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="21" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
-      <c r="E6" s="25"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="2">
         <v>0.73529999999999995</v>
       </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1898,7 +1971,7 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="19" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1907,51 +1980,51 @@
       <c r="G7" s="2">
         <v>0.78539999999999999</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="21">
         <v>16.601400000000002</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A8" s="25"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="2">
         <v>0.67610000000000003</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="31"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="E11" s="19" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="E11" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
@@ -1963,10 +2036,10 @@
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="23"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="3" t="s">
         <v>35</v>
       </c>
@@ -1987,7 +2060,7 @@
       <c r="C13" s="2">
         <v>5.0496999999999996</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1996,10 +2069,10 @@
       <c r="G13" s="2">
         <v>0.60419999999999996</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="21">
         <v>6.7031000000000001</v>
       </c>
-      <c r="I13" s="33" t="s">
+      <c r="I13" s="21" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2013,23 +2086,23 @@
       <c r="C14" s="2">
         <v>5.5609000000000002</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G14" s="2">
         <v>0.56520000000000004</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="32"/>
-      <c r="E15" s="24" t="s">
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="E15" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -2038,15 +2111,15 @@
       <c r="G15" s="2">
         <v>0.58009999999999995</v>
       </c>
-      <c r="H15" s="33">
+      <c r="H15" s="21">
         <v>2.8894000000000002</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="21">
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2055,25 +2128,25 @@
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="25"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="2">
         <v>0.5534</v>
       </c>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A17" s="25"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="19" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -2082,37 +2155,37 @@
       <c r="G17" s="2">
         <v>0.5393</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H17" s="21">
         <v>1.9854000000000001</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="21">
         <v>3.7600000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="E18" s="25"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="2">
         <v>0.52139999999999997</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
@@ -2148,14 +2221,14 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="34"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2166,7 +2239,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A26" s="25"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="2" t="s">
         <v>17</v>
       </c>
@@ -2176,24 +2249,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:E4"/>
@@ -2210,6 +2265,24 @@
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A24:C24"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2219,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2687A086-E6AD-4DC9-8E6D-5E9AEFD1DED8}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -2235,7 +2308,7 @@
     <col min="7" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="35" t="s">
         <v>41</v>
       </c>
@@ -2246,7 +2319,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="16" t="s">
         <v>39</v>
       </c>
@@ -2260,8 +2333,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2274,8 +2347,8 @@
         <v>34169</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="25"/>
+    <row r="4" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="20"/>
       <c r="B4" s="4" t="s">
         <v>68</v>
       </c>
@@ -2286,8 +2359,8 @@
         <v>17553</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2300,8 +2373,8 @@
         <v>19922</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="25"/>
+    <row r="6" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>68</v>
       </c>
@@ -2312,8 +2385,8 @@
         <v>40701</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2326,8 +2399,8 @@
         <v>13377</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="25"/>
+    <row r="8" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
         <v>68</v>
       </c>
@@ -2341,11 +2414,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="13"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="35" t="s">
         <v>65</v>
       </c>
@@ -2354,7 +2427,7 @@
       <c r="D10" s="36"/>
       <c r="E10" s="37"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="16" t="s">
         <v>39</v>
       </c>
@@ -2370,9 +2443,12 @@
       <c r="E11" s="16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="24" t="s">
+      <c r="G11" s="40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2392,8 +2468,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13" s="25"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
         <v>63</v>
       </c>
@@ -2410,9 +2486,13 @@
       <c r="F13" s="11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="24" t="s">
+      <c r="G13" s="1">
+        <f>ABS(E13-E12)</f>
+        <v>2.8600000000000014E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2432,8 +2512,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A15" s="25"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15" s="20"/>
       <c r="B15" s="4" t="s">
         <v>63</v>
       </c>
@@ -2450,9 +2530,13 @@
       <c r="F15" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A16" s="24" t="s">
+      <c r="G15" s="1">
+        <f>ABS(E15-E14)</f>
+        <v>3.8600000000000023E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2473,7 +2557,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A17" s="25"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>63</v>
       </c>
@@ -2489,6 +2573,10 @@
       </c>
       <c r="F17" s="11" t="s">
         <v>50</v>
+      </c>
+      <c r="G17" s="1">
+        <f>ABS(E17-E16)</f>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.5">
@@ -2518,7 +2606,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -2540,7 +2628,7 @@
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A22" s="25"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="4" t="s">
         <v>63</v>
       </c>
@@ -2557,10 +2645,14 @@
       <c r="F22" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="G22" s="1">
+        <f>ABS(E22-E21)</f>
+        <v>6.7799999999999999E-2</v>
+      </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2581,7 +2673,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A24" s="25"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="4" t="s">
         <v>63</v>
       </c>
@@ -2598,9 +2690,13 @@
       <c r="F24" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="G24" s="1">
+        <f>ABS(E24-E23)</f>
+        <v>0.15890000000000001</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2621,7 +2717,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A26" s="25"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="4" t="s">
         <v>63</v>
       </c>
@@ -2638,6 +2734,10 @@
       <c r="F26" s="6" t="s">
         <v>47</v>
       </c>
+      <c r="G26" s="1">
+        <f>ABS(E26-E25)</f>
+        <v>0.16839999999999999</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="E28" s="17" t="s">
@@ -2649,8 +2749,264 @@
         <v>70</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A32" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="37"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A33" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A34" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="42">
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="D34" s="42">
+        <v>0.9325</v>
+      </c>
+      <c r="E34" s="42">
+        <v>0.84360000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A35" s="43"/>
+      <c r="B35" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="42">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="D35" s="42">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="E35" s="42">
+        <v>0.8548</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A36" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="42">
+        <v>0.78420000000000001</v>
+      </c>
+      <c r="D36" s="42">
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="E36" s="42">
+        <v>0.79400000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A37" s="43"/>
+      <c r="B37" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="42">
+        <v>0.70940000000000003</v>
+      </c>
+      <c r="D37" s="42">
+        <v>0.79159999999999997</v>
+      </c>
+      <c r="E37" s="42">
+        <v>0.79369999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A38" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="42">
+        <v>0.88170000000000004</v>
+      </c>
+      <c r="D38" s="42">
+        <v>0.90090000000000003</v>
+      </c>
+      <c r="E38" s="42">
+        <v>0.81720000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A39" s="43"/>
+      <c r="B39" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="42">
+        <v>0.83930000000000005</v>
+      </c>
+      <c r="D39" s="42">
+        <v>0.87690000000000001</v>
+      </c>
+      <c r="E39" s="42">
+        <v>0.80720000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A40" s="42"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A41" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="49"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A42" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="47"/>
+      <c r="C42" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A43" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="42">
+        <v>0.8448</v>
+      </c>
+      <c r="D43" s="42">
+        <v>0.85640000000000005</v>
+      </c>
+      <c r="E43" s="42">
+        <v>0.81789999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A44" s="43"/>
+      <c r="B44" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="42">
+        <v>0.8296</v>
+      </c>
+      <c r="D44" s="42">
+        <v>0.85489999999999999</v>
+      </c>
+      <c r="E44" s="42">
+        <v>0.82050000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A45" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="42">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="D45" s="42">
+        <v>0.90490000000000004</v>
+      </c>
+      <c r="E45" s="42">
+        <v>0.82369999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A46" s="43"/>
+      <c r="B46" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="42">
+        <v>0.77</v>
+      </c>
+      <c r="D46" s="42">
+        <v>0.8286</v>
+      </c>
+      <c r="E46" s="42">
+        <v>0.80900000000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A47" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="42">
+        <v>0.82189999999999996</v>
+      </c>
+      <c r="D47" s="42">
+        <v>0.86229999999999996</v>
+      </c>
+      <c r="E47" s="42">
+        <v>0.80179999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A48" s="43"/>
+      <c r="B48" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="42">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D48" s="42">
+        <v>0.83389999999999997</v>
+      </c>
+      <c r="E48" s="42">
+        <v>0.77090000000000003</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="22">
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:E32"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>

</xml_diff>